<commit_message>
- no async -
</commit_message>
<xml_diff>
--- a/pasteFile.xlsx
+++ b/pasteFile.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>sn</t>
+  </si>
+  <si>
+    <t>Loc</t>
   </si>
   <si>
     <t>Tag no</t>
@@ -363,18 +366,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F2"/>
+  <dimension ref="A2:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="B3:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -392,9 +397,13 @@
       </c>
       <c r="F2" t="s">
         <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>